<commit_message>
Programas para limpar diretórios e informativos
</commit_message>
<xml_diff>
--- a/Files/5-16-18 GRE´s.xlsx
+++ b/Files/5-16-18 GRE´s.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="285" yWindow="195" windowWidth="7470" windowHeight="11760"/>
+    <workbookView xWindow="285" yWindow="195" windowWidth="7470" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="05º GRE " sheetId="3" r:id="rId1"/>
@@ -433,9 +433,6 @@
     <t>NNL-7286</t>
   </si>
   <si>
-    <t>KIQ-8720</t>
-  </si>
-  <si>
     <t>SÃO JULIÃO</t>
   </si>
   <si>
@@ -488,6 +485,9 @@
   </si>
   <si>
     <t>SIMÕES</t>
+  </si>
+  <si>
+    <t>KZQ-8720</t>
   </si>
 </sst>
 </file>
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,10 +1955,10 @@
     </row>
     <row r="11" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="51" t="s">
         <v>133</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>134</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>12</v>
@@ -1969,10 +1969,10 @@
     </row>
     <row r="12" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>5</v>
@@ -1983,13 +1983,13 @@
     </row>
     <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>136</v>
-      </c>
-      <c r="B13" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>137</v>
       </c>
       <c r="D13" s="52" t="s">
         <v>131</v>
@@ -1997,10 +1997,10 @@
     </row>
     <row r="14" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>6</v>
@@ -2011,10 +2011,10 @@
     </row>
     <row r="15" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>5</v>
@@ -2025,10 +2025,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>7</v>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>7</v>
@@ -2053,10 +2053,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>4</v>
@@ -2066,11 +2066,11 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>143</v>
+      <c r="A19" s="57" t="s">
+        <v>142</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>6</v>
@@ -2081,24 +2081,24 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>7</v>
@@ -2109,10 +2109,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B22" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>7</v>
@@ -2123,10 +2123,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B23" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>12</v>
@@ -2137,10 +2137,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>6</v>
@@ -2159,7 +2159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>